<commit_message>
LED bar replacement charges #CRMS-1638
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/Partner_invoice_detail_template-v2-open_cell.xlsx
+++ b/application/controllers/excel-templates/Partner_invoice_detail_template-v2-open_cell.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="25">
   <si>
     <t>ANNEXURE - Open Cell &amp; LED Bar Charges</t>
   </si>
@@ -67,15 +67,9 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Quantity</t>
-  </si>
-  <si>
     <t>Price</t>
   </si>
   <si>
-    <t>Spare ID</t>
-  </si>
-  <si>
     <t>{booking:order_id}</t>
   </si>
   <si>
@@ -85,19 +79,10 @@
     <t>{booking:description}</t>
   </si>
   <si>
-    <t>{booking:shipped_quantity}</t>
-  </si>
-  <si>
     <t>{booking:partner_charge}</t>
   </si>
   <si>
-    <t>{booking:spare_id}</t>
-  </si>
-  <si>
     <t>TOTAL</t>
-  </si>
-  <si>
-    <t>{meta:total_open_cell_quantity}</t>
   </si>
   <si>
     <t>{meta:total_open_cell_price}</t>
@@ -158,7 +143,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border/>
     <border>
       <left style="medium">
@@ -229,18 +214,7 @@
       <top/>
     </border>
     <border>
-      <right/>
       <top/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <bottom/>
-    </border>
-    <border>
-      <right/>
-      <bottom/>
     </border>
     <border>
       <left style="medium">
@@ -310,7 +284,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -371,33 +345,32 @@
     <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="12" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
     <xf borderId="8" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="13" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="14" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="15" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="11" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="12" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="14" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf borderId="15" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="16" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="17" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="18" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -620,9 +593,8 @@
     <col customWidth="1" min="2" max="2" width="14.43"/>
     <col customWidth="1" min="3" max="3" width="19.43"/>
     <col customWidth="1" min="4" max="4" width="18.14"/>
-    <col customWidth="1" min="5" max="5" width="30.29"/>
-    <col customWidth="1" min="6" max="6" width="31.29"/>
-    <col customWidth="1" min="7" max="7" width="43.29"/>
+    <col customWidth="1" min="5" max="5" width="31.29"/>
+    <col customWidth="1" min="6" max="6" width="43.29"/>
   </cols>
   <sheetData>
     <row r="1" ht="15.75" customHeight="1">
@@ -632,7 +604,6 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
     </row>
     <row r="2" ht="27.75" customHeight="1">
       <c r="A2" s="2"/>
@@ -642,8 +613,7 @@
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="5"/>
+      <c r="F2" s="5"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
@@ -651,8 +621,7 @@
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="8"/>
@@ -662,8 +631,7 @@
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="10"/>
@@ -673,8 +641,7 @@
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="12" t="s">
+      <c r="F5" s="12" t="s">
         <v>3</v>
       </c>
     </row>
@@ -686,8 +653,7 @@
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>5</v>
       </c>
     </row>
@@ -699,8 +665,7 @@
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="12" t="s">
+      <c r="F7" s="12" t="s">
         <v>7</v>
       </c>
     </row>
@@ -710,8 +675,7 @@
       <c r="C8" s="13"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="12"/>
+      <c r="F8" s="12"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="1"/>
@@ -719,8 +683,7 @@
       <c r="C9" s="13"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="14"/>
@@ -730,8 +693,7 @@
       <c r="C10" s="13"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>9</v>
       </c>
     </row>
@@ -743,8 +705,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="12" t="s">
+      <c r="F11" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -756,19 +717,16 @@
       <c r="C12" s="20"/>
       <c r="D12" s="21"/>
       <c r="E12" s="21"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="16" t="s">
+      <c r="F12" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="17"/>
       <c r="B13" s="22"/>
-      <c r="C13" s="23"/>
       <c r="D13" s="21"/>
       <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="16" t="s">
         <v>9</v>
       </c>
     </row>
@@ -780,59 +738,47 @@
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
       <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="24"/>
+      <c r="F14" s="23"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="21"/>
-      <c r="B15" s="25"/>
+      <c r="B15" s="24"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
       <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="24"/>
+      <c r="F15" s="23"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="21"/>
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="27" t="s">
+      <c r="D16" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="E16" s="27" t="s">
+      <c r="E16" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="F16" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>20</v>
-      </c>
+      <c r="F16" s="27"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="E17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="12" t="s">
-        <v>26</v>
-      </c>
+      <c r="F17" s="12"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="1"/>
@@ -840,23 +786,19 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="14"/>
-      <c r="B19" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="31" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="G19" s="32"/>
+      <c r="B19" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="29"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="31"/>
     </row>
     <row r="20" ht="15.75" customHeight="1"/>
     <row r="21" ht="15.75" customHeight="1"/>
@@ -1841,8 +1783,8 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="B2:G2"/>
     <mergeCell ref="B12:C13"/>
+    <mergeCell ref="B2:F2"/>
   </mergeCells>
   <printOptions/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>